<commit_message>
updated table extraction script to read multiple columns
</commit_message>
<xml_diff>
--- a/output/extracted_table.xlsx
+++ b/output/extracted_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,124 +434,264 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>Value_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Value_2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Value_3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Revenues $ 282,836 $ 307,394 $ 350,018</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>Revenues</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>282,836</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>307,394</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>350,018</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Costs and expenses:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Cost of revenues</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>126,203</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>133,332</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>146,306</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cost of revenues 126,203 133,332 146,306</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>Research and development</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>39,500</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>45,427</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>49,326</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Research and development 39,500 45,427 49,326</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>Sales and marketing</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>26,567</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>27,917</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>27,808</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sales and marketing 26,567 27,917 27,808</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
+          <t>General and administrative</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>15,724</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>16,425</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>14,188</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>General and administrative 15,724 16,425 14,188</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>Total costs and expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>207,994</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>223,101</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>237,628</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Total costs and expenses 207,994 223,101 237,628</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>Income from operations</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>74,842</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>84,293</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>112,390</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Income from operations 74,842 84,293 112,390</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
+          <t>Other income (expense), net (3,514)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1,424</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>7,425</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Other income (expense), net (3,514) 1,424 7,425</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
+          <t>Income before income taxes</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>71,328</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>85,717</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>119,815</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Income before income taxes 71,328 85,717 119,815</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
+          <t>Provision for income taxes</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11,356</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>11,922</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>19,697</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Provision for income taxes 11,356 11,922 19,697</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Net income $ 59,972 $ 73,795 $ 100,118</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Basic net income per share (Note 12) $ 4.59 $ 5.84 $ 8.13</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Diluted net income per share (Note 12) $ 4.56 $ 5.80 $ 8.04</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
+          <t>Net income</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>59,972</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>73,795</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>100,118</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated table reading to read negatives and notes
</commit_message>
<xml_diff>
--- a/output/extracted_table.xlsx
+++ b/output/extracted_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>282,836</t>
+          <t>282836</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>307,394</t>
+          <t>307394</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>350,018</t>
+          <t>350018</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>126,203</t>
+          <t>126203</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>133,332</t>
+          <t>133332</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>146,306</t>
+          <t>146306</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>39,500</t>
+          <t>39500</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>45,427</t>
+          <t>45427</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>49,326</t>
+          <t>49326</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>26,567</t>
+          <t>26567</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>27,917</t>
+          <t>27917</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>27,808</t>
+          <t>27808</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15,724</t>
+          <t>15724</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>16,425</t>
+          <t>16425</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14,188</t>
+          <t>14188</t>
         </is>
       </c>
     </row>
@@ -573,17 +573,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>207,994</t>
+          <t>207994</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>223,101</t>
+          <t>223101</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>237,628</t>
+          <t>237628</t>
         </is>
       </c>
     </row>
@@ -595,37 +595,41 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>74,842</t>
+          <t>74842</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>84,293</t>
+          <t>84293</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>112,390</t>
+          <t>112390</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Other income (expense), net (3,514)</t>
+          <t>Other income (expense), net</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1,424</t>
+          <t>-3514</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7,425</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>1424</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>7425</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -635,17 +639,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>71,328</t>
+          <t>71328</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>85,717</t>
+          <t>85717</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>119,815</t>
+          <t>119815</t>
         </is>
       </c>
     </row>
@@ -657,17 +661,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11,356</t>
+          <t>11356</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>11,922</t>
+          <t>11922</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>19,697</t>
+          <t>19697</t>
         </is>
       </c>
     </row>
@@ -679,17 +683,61 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>59,972</t>
+          <t>59972</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>73,795</t>
+          <t>73795</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>100,118</t>
+          <t>100118</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Basic net income per share (Note 12)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4.59</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>5.84</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>8.13</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Diluted net income per share (Note 12)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>4.56</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>5.80</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>8.04</t>
         </is>
       </c>
     </row>

</xml_diff>